<commit_message>
Re-instate api config value for merge. Fix missing product ID in Test data sheet. Add logging for custom listener steps.
</commit_message>
<xml_diff>
--- a/resources/testData/testData.xlsx
+++ b/resources/testData/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willyeng/Documents/ampion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willyeng/Source/auspost-javatestautomation/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC49907-4365-0A44-8ACD-54D5B8401848}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83070483-357C-B14F-8097-E80A586A03A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44160" yWindow="-5020" windowWidth="33600" windowHeight="20540" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOEExtension" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="101">
   <si>
     <t>T001_openBOEExtension</t>
   </si>
@@ -1638,7 +1638,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="248" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1892,13 +1892,16 @@
         <v>71</v>
       </c>
       <c r="E16" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
         <v>99</v>
       </c>
@@ -1908,15 +1911,16 @@
       <c r="D17" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="8"/>
+      <c r="F17" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="G18" t="s">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>